<commit_message>
refactor: ajuste no diagrama de classe e novamente no MER
</commit_message>
<xml_diff>
--- a/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
+++ b/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio" sheetId="1" r:id="rId1"/>
     <sheet name="Usuario" sheetId="2" r:id="rId2"/>
     <sheet name="Banco_Leite" sheetId="3" r:id="rId3"/>
-    <sheet name="Notificacao" sheetId="4" r:id="rId4"/>
+    <sheet name="Agendamento" sheetId="5" r:id="rId4"/>
+    <sheet name="Notificacao" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>Campo</t>
   </si>
@@ -203,13 +204,52 @@
   </si>
   <si>
     <t>Longitude da localização</t>
+  </si>
+  <si>
+    <t>Chave primária da tabela agendamento.</t>
+  </si>
+  <si>
+    <t>data_hora</t>
+  </si>
+  <si>
+    <t>Timestamptz</t>
+  </si>
+  <si>
+    <t>Data e hora do agendamento, com fuso horário.</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>Local do agendamento (endereço ou descrição do local).</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Status do agendamento (ex: pendente, confirmado, cancelado).</t>
+  </si>
+  <si>
+    <t>id_usuario</t>
+  </si>
+  <si>
+    <t>Usuário responsável pelo agendamento (chave estrangeira para usuário).</t>
+  </si>
+  <si>
+    <t>id_bancos_de_leite</t>
+  </si>
+  <si>
+    <t>Banco de leite relacionado ao agendamento (chave estrangeira para bancos_de_leite).</t>
+  </si>
+  <si>
+    <t>Tabela: Agendamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +267,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -275,17 +328,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -295,6 +341,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -612,12 +680,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -634,44 +702,44 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>100</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>100</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -701,12 +769,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -723,170 +791,170 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>100</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>100</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>100</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>8.6</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>8.6</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -904,7 +972,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,12 +984,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -938,100 +1006,100 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>100</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>255</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>20</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>8.6</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="4">
         <v>8.6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1045,10 +1113,144 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="54.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7">
+        <v>255</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,94 +1260,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: adicao e correção, questionário, cronograma, etc
</commit_message>
<xml_diff>
--- a/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
+++ b/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio" sheetId="1" r:id="rId1"/>
@@ -342,17 +342,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -361,7 +355,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -680,12 +680,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -769,12 +769,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,16 +980,16 @@
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1115,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1128,24 +1128,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1170,7 +1170,7 @@
       <c r="B4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1184,7 +1184,7 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>255</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1198,7 +1198,7 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1212,7 +1212,7 @@
       <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1226,7 +1226,7 @@
       <c r="B8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1234,7 +1234,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1260,94 +1260,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: correcoes no doc dicionario de dados
</commit_message>
<xml_diff>
--- a/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
+++ b/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC_2025_v38\PFC-DONATE\PFC_2025_Docs\ApêndiceD-VisãodosDados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6310A7-2736-47CD-9345-C82C93EF6F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Municipio" sheetId="1" r:id="rId1"/>
-    <sheet name="Usuario" sheetId="2" r:id="rId2"/>
-    <sheet name="Banco_Leite" sheetId="3" r:id="rId3"/>
-    <sheet name="Agendamento" sheetId="5" r:id="rId4"/>
-    <sheet name="Notificacao" sheetId="4" r:id="rId5"/>
+    <sheet name="municipio" sheetId="1" r:id="rId1"/>
+    <sheet name="unidade_federativa" sheetId="8" r:id="rId2"/>
+    <sheet name="token_recuperacao" sheetId="6" r:id="rId3"/>
+    <sheet name="usuario" sheetId="2" r:id="rId4"/>
+    <sheet name="banco_de_leite" sheetId="3" r:id="rId5"/>
+    <sheet name="doacao" sheetId="5" r:id="rId6"/>
+    <sheet name="evento" sheetId="7" r:id="rId7"/>
+    <sheet name="Notificacao" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
   <si>
     <t>Campo</t>
   </si>
@@ -119,12 +128,6 @@
     <t>Mensagem enviada.</t>
   </si>
   <si>
-    <t>Tabela: Usuário</t>
-  </si>
-  <si>
-    <t>Tabela: Banco_leite</t>
-  </si>
-  <si>
     <t>Tabela: Notificação</t>
   </si>
   <si>
@@ -185,9 +188,6 @@
     <t>Unidade federativa (Estado)</t>
   </si>
   <si>
-    <t>Tabela: Município</t>
-  </si>
-  <si>
     <t>Chave primária da tabela bancos_de_leite</t>
   </si>
   <si>
@@ -242,13 +242,94 @@
     <t>Banco de leite relacionado ao agendamento (chave estrangeira para bancos_de_leite).</t>
   </si>
   <si>
-    <t>Tabela: Agendamento</t>
+    <t>Tabela: banco_de_leite</t>
+  </si>
+  <si>
+    <t>Tabela: município</t>
+  </si>
+  <si>
+    <t>Tabela: usuario</t>
+  </si>
+  <si>
+    <t>Tabela: doacao</t>
+  </si>
+  <si>
+    <t>usuario_id</t>
+  </si>
+  <si>
+    <t>Usuario que esta solicitando a recuperação da senha</t>
+  </si>
+  <si>
+    <t>código de recuperação</t>
+  </si>
+  <si>
+    <t>data_expiracao</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>data de expiração do token</t>
+  </si>
+  <si>
+    <t>usado</t>
+  </si>
+  <si>
+    <t>Se o token foi utilizado ou não</t>
+  </si>
+  <si>
+    <t>Tabela: evento</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>Titulo do evento.</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>descricao do evento</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>data do evento</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>Definição do tipo do evento se é noticia ou evento</t>
+  </si>
+  <si>
+    <t>Relacionamento com o municipio, para saber qual municipio vai ser o evento</t>
+  </si>
+  <si>
+    <t>Tabela: unidade_federativa</t>
+  </si>
+  <si>
+    <t>sigla</t>
+  </si>
+  <si>
+    <t>Sigla Unidade federativa (Estado)</t>
+  </si>
+  <si>
+    <t>Nome da Unidade federativa</t>
+  </si>
+  <si>
+    <t>Tabela: usuario_token</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +433,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -374,14 +455,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -419,7 +503,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -491,7 +575,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,30 +748,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -712,10 +796,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -726,12 +810,12 @@
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -740,7 +824,7 @@
         <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -753,30 +837,228 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197DCA22-2CA9-413F-8127-6A67396CD86F}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J26:J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>255</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>255</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6345099A-8B81-42A0-A14C-433289CD0A47}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="65" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="B4:C14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +1072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -801,10 +1083,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -815,10 +1097,10 @@
         <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -829,10 +1111,10 @@
         <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -843,10 +1125,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -857,10 +1139,10 @@
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -871,10 +1153,10 @@
         <v>100</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -885,10 +1167,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -899,10 +1181,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -913,49 +1195,49 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3">
         <v>8.6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3">
         <v>8.6</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -967,31 +1249,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1016,10 +1298,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1030,24 +1312,24 @@
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1058,10 +1340,10 @@
         <v>255</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1072,35 +1354,35 @@
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4">
         <v>8.6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4">
         <v>8.6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1111,23 +1393,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="54.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
@@ -1135,7 +1417,7 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1160,26 +1442,26 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -1188,12 +1470,12 @@
         <v>255</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -1202,38 +1484,38 @@
         <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
     </row>
   </sheetData>
@@ -1245,29 +1527,159 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21386C2-7F7C-4EAE-AA95-8896393B1956}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
+        <v>255</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6">
+        <v>255</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
+        <v>255</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1281,7 +1693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1295,7 +1707,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -1309,7 +1721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -1337,7 +1749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
doc: ajustes no dicionario de dados
</commit_message>
<xml_diff>
--- a/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
+++ b/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC_2025_v38\PFC-DONATE\PFC_2025_Docs\ApêndiceD-VisãodosDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6310A7-2736-47CD-9345-C82C93EF6F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7F9AD2-5BD4-4B40-8DA1-E259C3E8DBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="municipio" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="banco_de_leite" sheetId="3" r:id="rId5"/>
     <sheet name="doacao" sheetId="5" r:id="rId6"/>
     <sheet name="evento" sheetId="7" r:id="rId7"/>
-    <sheet name="Notificacao" sheetId="4" r:id="rId8"/>
+    <sheet name="notificacao" sheetId="4" r:id="rId8"/>
+    <sheet name="usuario_senha_historico" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="103">
   <si>
     <t>Campo</t>
   </si>
@@ -324,6 +325,18 @@
   </si>
   <si>
     <t>Tabela: usuario_token</t>
+  </si>
+  <si>
+    <t>Tabela: usuario_senha_historico</t>
+  </si>
+  <si>
+    <t>data_alteracao</t>
+  </si>
+  <si>
+    <t>senha de acesso ao sistema criptografada que foi alterada</t>
+  </si>
+  <si>
+    <t>data de alteração da senha</t>
   </si>
 </sst>
 </file>
@@ -925,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6345099A-8B81-42A0-A14C-433289CD0A47}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1267,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D9"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1675,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,4 +1782,103 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6108AD95-615F-407F-AF52-BF38CAC3AF43}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: ajsute no beckend depois de ter feito o ajuste no nome da tabela banco_de_leite
</commit_message>
<xml_diff>
--- a/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
+++ b/PFC_2025_Docs/ApêndiceD-VisãodosDados/Dicionario_de_Dados_Donate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC_2025_v38\PFC-DONATE\PFC_2025_Docs\ApêndiceD-VisãodosDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7F9AD2-5BD4-4B40-8DA1-E259C3E8DBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2884EBA-8638-43D4-A70A-FE4CFFEEEE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="municipio" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,14 @@
     <sheet name="banco_de_leite" sheetId="3" r:id="rId5"/>
     <sheet name="doacao" sheetId="5" r:id="rId6"/>
     <sheet name="evento" sheetId="7" r:id="rId7"/>
-    <sheet name="notificacao" sheetId="4" r:id="rId8"/>
-    <sheet name="usuario_senha_historico" sheetId="9" r:id="rId9"/>
+    <sheet name="usuario_senha_historico" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
   <si>
     <t>Campo</t>
   </si>
@@ -87,49 +86,10 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>Int</t>
-  </si>
-  <si>
     <t>endereco</t>
   </si>
   <si>
-    <t>255</t>
-  </si>
-  <si>
-    <t>id_banco_leite</t>
-  </si>
-  <si>
     <t>codigo</t>
-  </si>
-  <si>
-    <t>datahora_envio</t>
-  </si>
-  <si>
-    <t>mensagem</t>
-  </si>
-  <si>
-    <t>DateTime</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Chave primária da tabela Notificacao.</t>
-  </si>
-  <si>
-    <t>Banco de leite relacionado (chave estrangeira).</t>
-  </si>
-  <si>
-    <t>Código da notificação.</t>
-  </si>
-  <si>
-    <t>Data e hora do envio.</t>
-  </si>
-  <si>
-    <t>Mensagem enviada.</t>
-  </si>
-  <si>
-    <t>Tabela: Notificação</t>
   </si>
   <si>
     <t>Chave primária da tabela usuario</t>
@@ -343,7 +303,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,19 +321,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -422,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -442,10 +389,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -453,9 +396,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -777,12 +717,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -809,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,12 +763,12 @@
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -837,7 +777,7 @@
         <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -863,12 +803,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -895,7 +835,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,12 +849,12 @@
         <v>255</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -923,7 +863,7 @@
         <v>255</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -948,12 +888,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -980,26 +920,26 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -1008,26 +948,26 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
@@ -1036,7 +976,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1064,12 +1004,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1096,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1110,7 +1050,7 @@
         <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1124,7 +1064,7 @@
         <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1138,7 +1078,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1152,7 +1092,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1166,7 +1106,7 @@
         <v>100</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1180,7 +1120,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1194,7 +1134,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1208,7 +1148,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1216,13 +1156,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3">
         <v>8.6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1230,27 +1170,27 @@
         <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3">
         <v>8.6</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1279,12 +1219,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1311,7 +1251,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,26 +1265,26 @@
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -1353,7 +1293,7 @@
         <v>255</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,7 +1307,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,13 +1315,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4">
         <v>8.6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,13 +1329,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4">
         <v>8.6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1423,12 +1363,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1455,26 +1395,26 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -1483,12 +1423,12 @@
         <v>255</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -1497,39 +1437,39 @@
         <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1557,12 +1497,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="A1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1589,12 +1529,12 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -1603,26 +1543,26 @@
         <v>255</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -1631,12 +1571,12 @@
         <v>255</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -1645,21 +1585,21 @@
         <v>255</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1671,120 +1611,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6108AD95-615F-407F-AF52-BF38CAC3AF43}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1798,12 +1624,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1830,21 +1656,21 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,21 +1684,21 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>